<commit_message>
+ABS() and ASC(), cleaned up use of Fixed Point variables
</commit_message>
<xml_diff>
--- a/Supported.xlsx
+++ b/Supported.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/don/go/src/github.com/navionguy/basicwasm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F9B170E-FE6D-7143-8F19-D9B9B03EF35F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7EBEA0F-65A6-4B48-885C-A2616FA94038}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9460" yWindow="2680" windowWidth="22680" windowHeight="15380" xr2:uid="{AA62892B-5570-A74D-BDA8-A103E896D107}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="190">
   <si>
     <t>Functions, Commands &amp; Statement</t>
   </si>
@@ -960,7 +960,7 @@
   <dimension ref="A1:E185"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -989,11 +989,29 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -1435,6 +1453,9 @@
         <v>12</v>
       </c>
       <c r="C76" t="s">
+        <v>12</v>
+      </c>
+      <c r="D76" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2048,15 +2069,15 @@
       </c>
       <c r="B185">
         <f t="shared" ref="B185:D185" si="0">COUNTA(B2:B184)</f>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C185">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D185">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
+missed IntDbl eval, more intrinsics
</commit_message>
<xml_diff>
--- a/Supported.xlsx
+++ b/Supported.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/don/go/src/github.com/navionguy/basicwasm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7EBEA0F-65A6-4B48-885C-A2616FA94038}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF5A3BA-A2E6-A247-A80D-9869C36E9F7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9460" yWindow="2680" windowWidth="22680" windowHeight="15380" xr2:uid="{AA62892B-5570-A74D-BDA8-A103E896D107}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="190">
   <si>
     <t>Functions, Commands &amp; Statement</t>
   </si>
@@ -960,7 +960,7 @@
   <dimension ref="A1:E185"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1017,6 +1017,15 @@
       <c r="A4" t="s">
         <v>7</v>
       </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -1056,6 +1065,15 @@
       <c r="A10" t="s">
         <v>14</v>
       </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -1075,6 +1093,15 @@
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>18</v>
+      </c>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -2069,15 +2096,15 @@
       </c>
       <c r="B185">
         <f t="shared" ref="B185:D185" si="0">COUNTA(B2:B184)</f>
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C185">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D185">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more intrinsics, evaluation clean up, tests
</commit_message>
<xml_diff>
--- a/Supported.xlsx
+++ b/Supported.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/don/go/src/github.com/navionguy/basicwasm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF5A3BA-A2E6-A247-A80D-9869C36E9F7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76FC3258-311C-B34A-896A-B45B9DBB2497}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9460" yWindow="2680" windowWidth="22680" windowHeight="15380" xr2:uid="{AA62892B-5570-A74D-BDA8-A103E896D107}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="190">
   <si>
     <t>Functions, Commands &amp; Statement</t>
   </si>
@@ -959,8 +959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{264AD530-8319-C14F-BA84-D94176E8A777}">
   <dimension ref="A1:E185"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1089,6 +1089,15 @@
       <c r="A13" t="s">
         <v>17</v>
       </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -1160,11 +1169,29 @@
       <c r="A23" t="s">
         <v>28</v>
       </c>
+      <c r="B23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>29</v>
       </c>
+      <c r="B24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
@@ -1175,16 +1202,43 @@
       <c r="A26" t="s">
         <v>31</v>
       </c>
+      <c r="B26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>32</v>
       </c>
+      <c r="B27" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>33</v>
       </c>
+      <c r="B28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
@@ -1327,6 +1381,15 @@
       <c r="A51" t="s">
         <v>56</v>
       </c>
+      <c r="B51" t="s">
+        <v>12</v>
+      </c>
+      <c r="C51" t="s">
+        <v>12</v>
+      </c>
+      <c r="D51" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
@@ -1603,83 +1666,110 @@
       <c r="A96" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B96" t="s">
+        <v>12</v>
+      </c>
+      <c r="C96" t="s">
+        <v>12</v>
+      </c>
+      <c r="D96" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B97" t="s">
+        <v>12</v>
+      </c>
+      <c r="C97" t="s">
+        <v>12</v>
+      </c>
+      <c r="D97" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B98" t="s">
+        <v>12</v>
+      </c>
+      <c r="C98" t="s">
+        <v>12</v>
+      </c>
+      <c r="D98" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>117</v>
       </c>
@@ -2096,15 +2186,15 @@
       </c>
       <c r="B185">
         <f t="shared" ref="B185:D185" si="0">COUNTA(B2:B184)</f>
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C185">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="D185">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more intrinsics, execution tweeks, unit test love for lexer
</commit_message>
<xml_diff>
--- a/Supported.xlsx
+++ b/Supported.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/don/go/src/github.com/navionguy/basicwasm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76FC3258-311C-B34A-896A-B45B9DBB2497}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1905F415-998D-F54E-BF89-DE181151C181}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9460" yWindow="2680" windowWidth="22680" windowHeight="15380" xr2:uid="{AA62892B-5570-A74D-BDA8-A103E896D107}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="193">
   <si>
     <t>Functions, Commands &amp; Statement</t>
   </si>
@@ -603,6 +603,15 @@
   </si>
   <si>
     <t>WRITE#</t>
+  </si>
+  <si>
+    <t>No way to implement</t>
+  </si>
+  <si>
+    <t>returns 0 until printing is working</t>
+  </si>
+  <si>
+    <t>function, not statement</t>
   </si>
 </sst>
 </file>
@@ -959,8 +968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{264AD530-8319-C14F-BA84-D94176E8A777}">
   <dimension ref="A1:E185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="B149" sqref="B149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1367,17 +1376,17 @@
         <v>53</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>56</v>
       </c>
@@ -1391,42 +1400,51 @@
         <v>12</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
+        <v>12</v>
+      </c>
+      <c r="C55" t="s">
+        <v>12</v>
+      </c>
+      <c r="D55" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>64</v>
       </c>
@@ -1437,7 +1455,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>65</v>
       </c>
@@ -1451,12 +1469,21 @@
         <v>12</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B61" t="s">
+        <v>12</v>
+      </c>
+      <c r="C61" t="s">
+        <v>12</v>
+      </c>
+      <c r="D61" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>67</v>
       </c>
@@ -1470,14 +1497,26 @@
         <v>12</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B63" t="s">
+        <v>12</v>
+      </c>
+      <c r="C63" t="s">
+        <v>12</v>
+      </c>
+      <c r="D63" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>69</v>
+      </c>
+      <c r="E64" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
@@ -1499,11 +1538,29 @@
       <c r="A68" t="s">
         <v>73</v>
       </c>
+      <c r="B68" t="s">
+        <v>12</v>
+      </c>
+      <c r="C68" t="s">
+        <v>12</v>
+      </c>
+      <c r="D68" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>74</v>
       </c>
+      <c r="B69" t="s">
+        <v>12</v>
+      </c>
+      <c r="C69" t="s">
+        <v>12</v>
+      </c>
+      <c r="D69" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
@@ -1534,6 +1591,15 @@
       <c r="A75" t="s">
         <v>80</v>
       </c>
+      <c r="B75" t="s">
+        <v>12</v>
+      </c>
+      <c r="C75" t="s">
+        <v>12</v>
+      </c>
+      <c r="D75" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
@@ -1578,7 +1644,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>86</v>
       </c>
@@ -1592,77 +1658,110 @@
         <v>12</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B88" t="s">
+        <v>12</v>
+      </c>
+      <c r="C88" t="s">
+        <v>12</v>
+      </c>
+      <c r="D88" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B89" t="s">
+        <v>12</v>
+      </c>
+      <c r="C89" t="s">
+        <v>12</v>
+      </c>
+      <c r="D89" t="s">
+        <v>12</v>
+      </c>
+      <c r="E89" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B94" t="s">
+        <v>12</v>
+      </c>
+      <c r="C94" t="s">
+        <v>12</v>
+      </c>
+      <c r="D94" t="s">
+        <v>12</v>
+      </c>
+      <c r="E94" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>101</v>
       </c>
@@ -1723,6 +1822,15 @@
       <c r="A102" t="s">
         <v>107</v>
       </c>
+      <c r="B102" t="s">
+        <v>12</v>
+      </c>
+      <c r="C102" t="s">
+        <v>12</v>
+      </c>
+      <c r="D102" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
@@ -1946,6 +2054,15 @@
       <c r="A143" t="s">
         <v>149</v>
       </c>
+      <c r="B143" t="s">
+        <v>12</v>
+      </c>
+      <c r="C143" t="s">
+        <v>12</v>
+      </c>
+      <c r="D143" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
@@ -1955,6 +2072,15 @@
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>150</v>
+      </c>
+      <c r="B145" t="s">
+        <v>12</v>
+      </c>
+      <c r="C145" t="s">
+        <v>12</v>
+      </c>
+      <c r="D145" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
@@ -2186,15 +2312,15 @@
       </c>
       <c r="B185">
         <f t="shared" ref="B185:D185" si="0">COUNTA(B2:B184)</f>
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="C185">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="D185">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
last rounds of intrinsics, 28% language coverage
</commit_message>
<xml_diff>
--- a/Supported.xlsx
+++ b/Supported.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/don/go/src/github.com/navionguy/basicwasm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1905F415-998D-F54E-BF89-DE181151C181}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAE93B27-6FBD-9F45-A840-F58BC6B27235}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9460" yWindow="2680" windowWidth="22680" windowHeight="15380" xr2:uid="{AA62892B-5570-A74D-BDA8-A103E896D107}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="192">
   <si>
     <t>Functions, Commands &amp; Statement</t>
   </si>
@@ -524,9 +524,6 @@
     <t>SQR()</t>
   </si>
   <si>
-    <t>SOR()</t>
-  </si>
-  <si>
     <t>STICK()</t>
   </si>
   <si>
@@ -557,9 +554,6 @@
     <t>TIME$</t>
   </si>
   <si>
-    <t>TIMER()</t>
-  </si>
-  <si>
     <t>TROFF</t>
   </si>
   <si>
@@ -612,13 +606,23 @@
   </si>
   <si>
     <t>function, not statement</t>
+  </si>
+  <si>
+    <t>TIMER</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -644,17 +648,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -968,8 +975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{264AD530-8319-C14F-BA84-D94176E8A777}">
   <dimension ref="A1:E185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="B149" sqref="B149"/>
+    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="B185" sqref="B185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1516,7 +1523,7 @@
         <v>69</v>
       </c>
       <c r="E64" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
@@ -1716,7 +1723,7 @@
         <v>12</v>
       </c>
       <c r="E89" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
@@ -1753,7 +1760,7 @@
         <v>12</v>
       </c>
       <c r="E94" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
@@ -2111,6 +2118,15 @@
       <c r="A149" t="s">
         <v>154</v>
       </c>
+      <c r="B149" t="s">
+        <v>12</v>
+      </c>
+      <c r="C149" t="s">
+        <v>12</v>
+      </c>
+      <c r="D149" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
@@ -2121,6 +2137,15 @@
       <c r="A151" t="s">
         <v>157</v>
       </c>
+      <c r="B151" t="s">
+        <v>12</v>
+      </c>
+      <c r="C151" t="s">
+        <v>12</v>
+      </c>
+      <c r="D151" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
@@ -2131,6 +2156,15 @@
       <c r="A153" t="s">
         <v>158</v>
       </c>
+      <c r="B153" t="s">
+        <v>12</v>
+      </c>
+      <c r="C153" t="s">
+        <v>12</v>
+      </c>
+      <c r="D153" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
@@ -2141,6 +2175,15 @@
       <c r="A155" t="s">
         <v>160</v>
       </c>
+      <c r="B155" t="s">
+        <v>12</v>
+      </c>
+      <c r="C155" t="s">
+        <v>12</v>
+      </c>
+      <c r="D155" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
@@ -2151,6 +2194,15 @@
       <c r="A157" t="s">
         <v>162</v>
       </c>
+      <c r="B157" t="s">
+        <v>12</v>
+      </c>
+      <c r="C157" t="s">
+        <v>12</v>
+      </c>
+      <c r="D157" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
@@ -2166,6 +2218,15 @@
       <c r="A160" t="s">
         <v>165</v>
       </c>
+      <c r="B160" t="s">
+        <v>12</v>
+      </c>
+      <c r="C160" t="s">
+        <v>12</v>
+      </c>
+      <c r="D160" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
@@ -2176,6 +2237,15 @@
       <c r="A162" t="s">
         <v>167</v>
       </c>
+      <c r="B162" t="s">
+        <v>12</v>
+      </c>
+      <c r="C162" t="s">
+        <v>12</v>
+      </c>
+      <c r="D162" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
@@ -2196,6 +2266,15 @@
       <c r="A166" t="s">
         <v>171</v>
       </c>
+      <c r="B166" t="s">
+        <v>12</v>
+      </c>
+      <c r="C166" t="s">
+        <v>12</v>
+      </c>
+      <c r="D166" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
@@ -2204,17 +2283,26 @@
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>173</v>
+        <v>191</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>174</v>
+        <v>173</v>
+      </c>
+      <c r="B169" t="s">
+        <v>12</v>
+      </c>
+      <c r="C169" t="s">
+        <v>12</v>
+      </c>
+      <c r="D169" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B170" t="s">
         <v>12</v>
@@ -2228,99 +2316,108 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>176</v>
-      </c>
-      <c r="B171" t="s">
-        <v>12</v>
-      </c>
-      <c r="C171" t="s">
-        <v>12</v>
-      </c>
-      <c r="D171" t="s">
-        <v>12</v>
+        <v>175</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>178</v>
+        <v>177</v>
+      </c>
+      <c r="B173" t="s">
+        <v>12</v>
+      </c>
+      <c r="C173" t="s">
+        <v>12</v>
+      </c>
+      <c r="D173" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A184" t="s">
-        <v>189</v>
+      <c r="A184">
+        <f>COUNTA(A2:A183)</f>
+        <v>182</v>
+      </c>
+      <c r="B184">
+        <f t="shared" ref="B184:D184" si="0">COUNTA(B2:B183)</f>
+        <v>52</v>
+      </c>
+      <c r="C184">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="D184">
+        <f t="shared" si="0"/>
+        <v>51</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A185">
-        <f>COUNTA(A2:A184)</f>
-        <v>183</v>
-      </c>
-      <c r="B185">
-        <f t="shared" ref="B185:D185" si="0">COUNTA(B2:B184)</f>
-        <v>43</v>
-      </c>
-      <c r="C185">
-        <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
-      <c r="D185">
-        <f t="shared" si="0"/>
-        <v>42</v>
+      <c r="B185" s="2">
+        <f>B184/$A184</f>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="C185" s="2">
+        <f t="shared" ref="C185:D185" si="1">C184/$A184</f>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="D185" s="2">
+        <f t="shared" si="1"/>
+        <v>0.28021978021978022</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hex and octal constants
</commit_message>
<xml_diff>
--- a/Supported.xlsx
+++ b/Supported.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/don/go/src/github.com/navionguy/basicwasm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAE93B27-6FBD-9F45-A840-F58BC6B27235}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD478E2-BB31-2846-B29F-4E7E9DA70B42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9460" yWindow="2680" windowWidth="22680" windowHeight="15380" xr2:uid="{AA62892B-5570-A74D-BDA8-A103E896D107}"/>
+    <workbookView xWindow="40040" yWindow="2500" windowWidth="22680" windowHeight="15380" xr2:uid="{AA62892B-5570-A74D-BDA8-A103E896D107}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -615,7 +615,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -630,13 +630,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -648,18 +660,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -975,8 +990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{264AD530-8319-C14F-BA84-D94176E8A777}">
   <dimension ref="A1:E185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
-      <selection activeCell="B185" sqref="B185"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1066,16 +1081,25 @@
       <c r="A7" t="s">
         <v>9</v>
       </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>13</v>
       </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">

</xml_diff>

<commit_message>
added support for the DATA statement, cleaned up array logic
</commit_message>
<xml_diff>
--- a/Supported.xlsx
+++ b/Supported.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/don/go/src/github.com/navionguy/basicwasm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD478E2-BB31-2846-B29F-4E7E9DA70B42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01DBF454-E83F-7F46-9827-8ECD91752E9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40040" yWindow="2500" windowWidth="22680" windowHeight="15380" xr2:uid="{AA62892B-5570-A74D-BDA8-A103E896D107}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="192">
   <si>
     <t>Functions, Commands &amp; Statement</t>
   </si>
@@ -990,8 +990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{264AD530-8319-C14F-BA84-D94176E8A777}">
   <dimension ref="A1:E185"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1284,6 +1284,15 @@
       <c r="A29" t="s">
         <v>34</v>
       </c>
+      <c r="B29" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
@@ -2419,29 +2428,29 @@
       </c>
       <c r="B184">
         <f t="shared" ref="B184:D184" si="0">COUNTA(B2:B183)</f>
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C184">
         <f t="shared" si="0"/>
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D184">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B185" s="2">
         <f>B184/$A184</f>
-        <v>0.2857142857142857</v>
+        <v>0.29120879120879123</v>
       </c>
       <c r="C185" s="2">
         <f t="shared" ref="C185:D185" si="1">C184/$A184</f>
-        <v>0.2857142857142857</v>
+        <v>0.29120879120879123</v>
       </c>
       <c r="D185" s="2">
         <f t="shared" si="1"/>
-        <v>0.28021978021978022</v>
+        <v>0.2857142857142857</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
starting down the road to add support for chain, load, files and such
</commit_message>
<xml_diff>
--- a/Supported.xlsx
+++ b/Supported.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/don/go/src/github.com/navionguy/basicwasm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{988871D5-635D-CA4B-A671-4C18CEE70849}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{954B0604-95E9-E941-8EB4-73ED077AE83E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40040" yWindow="2500" windowWidth="22680" windowHeight="15380" xr2:uid="{AA62892B-5570-A74D-BDA8-A103E896D107}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{AA62892B-5570-A74D-BDA8-A103E896D107}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1005,8 +1005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{264AD530-8319-C14F-BA84-D94176E8A777}">
   <dimension ref="A1:E185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="D140" sqref="D140"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="H178" sqref="H178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2195,7 +2195,7 @@
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A150" t="s">
+      <c r="A150" s="4" t="s">
         <v>155</v>
       </c>
     </row>
@@ -2408,11 +2408,17 @@
       <c r="A174" t="s">
         <v>178</v>
       </c>
+      <c r="B174" s="3"/>
+      <c r="C174" s="3"/>
+      <c r="D174" s="3"/>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>179</v>
       </c>
+      <c r="B175" s="3"/>
+      <c r="C175" s="3"/>
+      <c r="D175" s="3"/>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A176" t="s">

</xml_diff>

<commit_message>
moved file requests to pacage fileserv
</commit_message>
<xml_diff>
--- a/Supported.xlsx
+++ b/Supported.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/don/go/src/github.com/navionguy/basicwasm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{954B0604-95E9-E941-8EB4-73ED077AE83E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{450492DC-50B2-FD4D-BB04-3AF03171A68C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{AA62892B-5570-A74D-BDA8-A103E896D107}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19000" xr2:uid="{AA62892B-5570-A74D-BDA8-A103E896D107}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="193">
   <si>
     <t>Functions, Commands &amp; Statement</t>
   </si>
@@ -609,6 +609,9 @@
   </si>
   <si>
     <t>TIMER</t>
+  </si>
+  <si>
+    <t>Token File</t>
   </si>
 </sst>
 </file>
@@ -1003,18 +1006,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{264AD530-8319-C14F-BA84-D94176E8A777}">
-  <dimension ref="A1:E185"/>
+  <dimension ref="A1:F185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="H178" sqref="H178"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="17280" ySplit="1800" topLeftCell="M27"/>
+      <selection activeCell="E1" sqref="E1"/>
+      <selection pane="topRight" activeCell="M1" sqref="M1"/>
+      <selection pane="bottomLeft" activeCell="D54" sqref="D54"/>
+      <selection pane="bottomRight" activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1028,10 +1035,13 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>192</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1045,7 +1055,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1059,7 +1069,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1073,7 +1083,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1087,36 +1097,39 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1130,17 +1143,17 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1154,7 +1167,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1168,22 +1181,22 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1196,31 +1209,31 @@
       <c r="D18" t="s">
         <v>12</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -1234,7 +1247,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -1248,12 +1261,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -1267,7 +1280,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -1281,7 +1294,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -1295,7 +1308,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -1309,12 +1322,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>36</v>
       </c>
@@ -1328,7 +1341,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -1431,17 +1444,17 @@
         <v>53</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>56</v>
       </c>
@@ -1455,22 +1468,31 @@
         <v>12</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
+        <v>12</v>
+      </c>
+      <c r="C54" t="s">
+        <v>12</v>
+      </c>
+      <c r="D54" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>60</v>
       </c>
@@ -1484,22 +1506,22 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
         <v>64</v>
       </c>
@@ -1510,7 +1532,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>65</v>
       </c>
@@ -1524,7 +1546,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>66</v>
       </c>
@@ -1538,7 +1560,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>67</v>
       </c>
@@ -1552,7 +1574,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>68</v>
       </c>
@@ -1566,11 +1588,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>69</v>
       </c>
-      <c r="E64" t="s">
+      <c r="F64" t="s">
         <v>188</v>
       </c>
     </row>
@@ -1699,7 +1721,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>86</v>
       </c>
@@ -1713,37 +1735,37 @@
         <v>12</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>93</v>
       </c>
@@ -1757,7 +1779,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>94</v>
       </c>
@@ -1770,31 +1792,31 @@
       <c r="D89" t="s">
         <v>12</v>
       </c>
-      <c r="E89" t="s">
+      <c r="F89" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>99</v>
       </c>
@@ -1807,16 +1829,16 @@
       <c r="D94" t="s">
         <v>12</v>
       </c>
-      <c r="E94" t="s">
+      <c r="F94" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>101</v>
       </c>
@@ -2294,12 +2316,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>167</v>
       </c>
@@ -2313,22 +2335,22 @@
         <v>12</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>171</v>
       </c>
@@ -2342,17 +2364,17 @@
         <v>12</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>173</v>
       </c>
@@ -2366,7 +2388,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>174</v>
       </c>
@@ -2380,17 +2402,17 @@
         <v>12</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>177</v>
       </c>
@@ -2404,93 +2426,96 @@
         <v>12</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>178</v>
       </c>
       <c r="B174" s="3"/>
       <c r="C174" s="3"/>
       <c r="D174" s="3"/>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E174" s="3"/>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>179</v>
       </c>
       <c r="B175" s="3"/>
       <c r="C175" s="3"/>
       <c r="D175" s="3"/>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E175" s="3"/>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184">
         <f>COUNTA(A2:A183)</f>
         <v>182</v>
       </c>
       <c r="B184">
         <f t="shared" ref="B184:D184" si="0">COUNTA(B2:B183)</f>
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C184">
         <f t="shared" si="0"/>
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D184">
         <f t="shared" si="0"/>
-        <v>54</v>
-      </c>
-    </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B185" s="2">
         <f>B184/$A184</f>
-        <v>0.30219780219780218</v>
+        <v>0.30769230769230771</v>
       </c>
       <c r="C185" s="2">
         <f t="shared" ref="C185:D185" si="1">C184/$A184</f>
-        <v>0.30219780219780218</v>
+        <v>0.30769230769230771</v>
       </c>
       <c r="D185" s="2">
         <f t="shared" si="1"/>
-        <v>0.2967032967032967</v>
-      </c>
+        <v>0.30219780219780218</v>
+      </c>
+      <c r="E185" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
finished loading of authentic gwbasic source files
</commit_message>
<xml_diff>
--- a/Supported.xlsx
+++ b/Supported.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/don/go/src/github.com/navionguy/basicwasm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{450492DC-50B2-FD4D-BB04-3AF03171A68C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0420372B-C9FB-AE4B-9625-CB8E0CFFCF55}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19000" xr2:uid="{AA62892B-5570-A74D-BDA8-A103E896D107}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="195">
   <si>
     <t>Functions, Commands &amp; Statement</t>
   </si>
@@ -419,9 +419,6 @@
     <t>PLAY</t>
   </si>
   <si>
-    <t>PLAN()</t>
-  </si>
-  <si>
     <t>PMAP</t>
   </si>
   <si>
@@ -612,6 +609,15 @@
   </si>
   <si>
     <t>Token File</t>
+  </si>
+  <si>
+    <t>options</t>
+  </si>
+  <si>
+    <t>spelled out</t>
+  </si>
+  <si>
+    <t>PLAY()</t>
   </si>
 </sst>
 </file>
@@ -1009,10 +1015,10 @@
   <dimension ref="A1:F185"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="17280" ySplit="1800" topLeftCell="M27"/>
+      <pane xSplit="17280" ySplit="1800" topLeftCell="M1" activePane="bottomLeft"/>
       <selection activeCell="E1" sqref="E1"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="D54" sqref="D54"/>
+      <selection pane="bottomLeft" activeCell="H172" sqref="H172"/>
       <selection pane="bottomRight" activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
@@ -1035,7 +1041,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -1054,6 +1060,9 @@
       <c r="D2" t="s">
         <v>12</v>
       </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -1068,6 +1077,9 @@
       <c r="D3" t="s">
         <v>12</v>
       </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -1082,6 +1094,9 @@
       <c r="D4" t="s">
         <v>12</v>
       </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -1096,11 +1111,26 @@
       <c r="D5" t="s">
         <v>12</v>
       </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -1109,7 +1139,9 @@
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -1118,7 +1150,9 @@
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -1127,7 +1161,9 @@
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -1142,16 +1178,37 @@
       <c r="D10" t="s">
         <v>12</v>
       </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
+      <c r="E12" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -1166,6 +1223,9 @@
       <c r="D13" t="s">
         <v>12</v>
       </c>
+      <c r="E13" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -1180,21 +1240,33 @@
       <c r="D14" t="s">
         <v>12</v>
       </c>
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>19</v>
       </c>
+      <c r="E15" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>20</v>
       </c>
+      <c r="E16" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>21</v>
       </c>
+      <c r="E17" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
@@ -1209,6 +1281,9 @@
       <c r="D18" t="s">
         <v>12</v>
       </c>
+      <c r="E18" t="s">
+        <v>12</v>
+      </c>
       <c r="F18" t="s">
         <v>23</v>
       </c>
@@ -1217,21 +1292,33 @@
       <c r="A19" s="4" t="s">
         <v>24</v>
       </c>
+      <c r="E19" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>25</v>
       </c>
+      <c r="E20" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>26</v>
       </c>
+      <c r="E21" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>27</v>
       </c>
+      <c r="E22" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
@@ -1246,6 +1333,9 @@
       <c r="D23" t="s">
         <v>12</v>
       </c>
+      <c r="E23" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
@@ -1260,11 +1350,23 @@
       <c r="D24" t="s">
         <v>12</v>
       </c>
+      <c r="E24" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>30</v>
       </c>
+      <c r="B25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
@@ -1279,6 +1381,9 @@
       <c r="D26" t="s">
         <v>12</v>
       </c>
+      <c r="E26" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
@@ -1293,6 +1398,9 @@
       <c r="D27" t="s">
         <v>12</v>
       </c>
+      <c r="E27" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
@@ -1307,6 +1415,9 @@
       <c r="D28" t="s">
         <v>12</v>
       </c>
+      <c r="E28" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
@@ -1321,11 +1432,17 @@
       <c r="D29" t="s">
         <v>12</v>
       </c>
+      <c r="E29" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>35</v>
       </c>
+      <c r="E30" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
@@ -1340,43 +1457,70 @@
       <c r="D31" t="s">
         <v>12</v>
       </c>
+      <c r="E31" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E32" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E33" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E34" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E35" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E36" t="s">
+        <v>12</v>
+      </c>
+      <c r="F36" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E37" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E38" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>44</v>
       </c>
@@ -1389,18 +1533,27 @@
       <c r="D39" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E39" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E40" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E41" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>47</v>
       </c>
@@ -1413,46 +1566,73 @@
       <c r="D42" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E42" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E43" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E44" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E45" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E46" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E47" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>53</v>
+      </c>
+      <c r="E48" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>54</v>
       </c>
+      <c r="E49" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>55</v>
       </c>
+      <c r="E50" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
@@ -1467,16 +1647,25 @@
       <c r="D51" t="s">
         <v>12</v>
       </c>
+      <c r="E51" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>57</v>
       </c>
+      <c r="E52" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>58</v>
       </c>
+      <c r="E53" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
@@ -1491,6 +1680,9 @@
       <c r="D54" t="s">
         <v>12</v>
       </c>
+      <c r="E54" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
@@ -1505,21 +1697,33 @@
       <c r="D55" t="s">
         <v>12</v>
       </c>
+      <c r="E55" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>61</v>
       </c>
+      <c r="E56" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>62</v>
       </c>
+      <c r="E57" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>63</v>
       </c>
+      <c r="E58" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
@@ -1531,6 +1735,9 @@
       <c r="C59" t="s">
         <v>12</v>
       </c>
+      <c r="E59" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
@@ -1545,6 +1752,9 @@
       <c r="D60" t="s">
         <v>12</v>
       </c>
+      <c r="E60" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
@@ -1559,6 +1769,9 @@
       <c r="D61" t="s">
         <v>12</v>
       </c>
+      <c r="E61" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
@@ -1573,6 +1786,9 @@
       <c r="D62" t="s">
         <v>12</v>
       </c>
+      <c r="E62" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
@@ -1587,31 +1803,46 @@
       <c r="D63" t="s">
         <v>12</v>
       </c>
+      <c r="E63" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>69</v>
       </c>
+      <c r="E64" t="s">
+        <v>12</v>
+      </c>
       <c r="F64" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E65" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E66" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E67" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>73</v>
       </c>
@@ -1624,8 +1855,11 @@
       <c r="D68" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E68" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>74</v>
       </c>
@@ -1638,33 +1872,51 @@
       <c r="D69" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E69" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E70" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E71" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E72" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E73" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E74" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>80</v>
       </c>
@@ -1677,8 +1929,11 @@
       <c r="D75" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E75" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>81</v>
       </c>
@@ -1691,8 +1946,11 @@
       <c r="D76" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E76" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>82</v>
       </c>
@@ -1705,20 +1963,32 @@
       <c r="D77" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E77" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E78" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E79" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>85</v>
+      </c>
+      <c r="E80" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
@@ -1734,36 +2004,57 @@
       <c r="D81" t="s">
         <v>12</v>
       </c>
+      <c r="E81" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>87</v>
       </c>
+      <c r="E82" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>88</v>
       </c>
+      <c r="E83" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>89</v>
       </c>
+      <c r="E84" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
         <v>90</v>
       </c>
+      <c r="E85" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>91</v>
       </c>
+      <c r="E86" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>92</v>
       </c>
+      <c r="E87" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
@@ -1778,6 +2069,9 @@
       <c r="D88" t="s">
         <v>12</v>
       </c>
+      <c r="E88" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
@@ -1792,29 +2086,44 @@
       <c r="D89" t="s">
         <v>12</v>
       </c>
+      <c r="E89" t="s">
+        <v>12</v>
+      </c>
       <c r="F89" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>95</v>
       </c>
+      <c r="E90" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>96</v>
       </c>
+      <c r="E91" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>97</v>
       </c>
+      <c r="E92" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>98</v>
       </c>
+      <c r="E93" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
@@ -1829,14 +2138,20 @@
       <c r="D94" t="s">
         <v>12</v>
       </c>
+      <c r="E94" t="s">
+        <v>12</v>
+      </c>
       <c r="F94" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>100</v>
       </c>
+      <c r="E95" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
@@ -1851,8 +2166,11 @@
       <c r="D96" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E96" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>102</v>
       </c>
@@ -1865,8 +2183,11 @@
       <c r="D97" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E97" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>103</v>
       </c>
@@ -1879,23 +2200,35 @@
       <c r="D98" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E98" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E99" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E100" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E101" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>107</v>
       </c>
@@ -1908,404 +2241,578 @@
       <c r="D102" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E102" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E103" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E104" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E105" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E106" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E107" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E108" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E109" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E110" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E111" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="E112" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="E113" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="E114" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="E115" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="E116" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="E117" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="E118" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="E119" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="E120" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="E121" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="E122" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
+        <v>194</v>
+      </c>
+      <c r="E123" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A124" t="s">
+      <c r="E124" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A125" t="s">
+      <c r="E125" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A126" t="s">
+      <c r="E126" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A127" t="s">
+      <c r="E127" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A128" t="s">
+      <c r="E128" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A129" t="s">
+      <c r="E129" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A130" t="s">
+      <c r="B130" t="s">
+        <v>12</v>
+      </c>
+      <c r="C130" t="s">
+        <v>12</v>
+      </c>
+      <c r="D130" t="s">
+        <v>12</v>
+      </c>
+      <c r="E130" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
         <v>135</v>
       </c>
-      <c r="B130" t="s">
-        <v>12</v>
-      </c>
-      <c r="C130" t="s">
-        <v>12</v>
-      </c>
-      <c r="D130" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A131" t="s">
+      <c r="E131" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A132" t="s">
+      <c r="E132" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A133" t="s">
+      <c r="E133" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A134" t="s">
+      <c r="E134" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A135" t="s">
+      <c r="E135" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A136" t="s">
+      <c r="B136" t="s">
+        <v>12</v>
+      </c>
+      <c r="C136" t="s">
+        <v>12</v>
+      </c>
+      <c r="D136" t="s">
+        <v>12</v>
+      </c>
+      <c r="E136" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
         <v>141</v>
       </c>
-      <c r="B136" t="s">
-        <v>12</v>
-      </c>
-      <c r="C136" t="s">
-        <v>12</v>
-      </c>
-      <c r="D136" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A137" t="s">
+      <c r="B137" t="s">
+        <v>12</v>
+      </c>
+      <c r="C137" t="s">
+        <v>12</v>
+      </c>
+      <c r="D137" t="s">
+        <v>12</v>
+      </c>
+      <c r="E137" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
         <v>142</v>
       </c>
-      <c r="B137" t="s">
-        <v>12</v>
-      </c>
-      <c r="C137" t="s">
-        <v>12</v>
-      </c>
-      <c r="D137" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A138" t="s">
+      <c r="E138" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A139" t="s">
+      <c r="E139" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A140" t="s">
+      <c r="B140" t="s">
+        <v>12</v>
+      </c>
+      <c r="C140" t="s">
+        <v>12</v>
+      </c>
+      <c r="D140" t="s">
+        <v>12</v>
+      </c>
+      <c r="E140" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
         <v>145</v>
       </c>
-      <c r="B140" t="s">
-        <v>12</v>
-      </c>
-      <c r="C140" t="s">
-        <v>12</v>
-      </c>
-      <c r="D140" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A141" t="s">
+      <c r="E141" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A142" t="s">
+      <c r="E142" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>148</v>
+      </c>
+      <c r="B143" t="s">
+        <v>12</v>
+      </c>
+      <c r="C143" t="s">
+        <v>12</v>
+      </c>
+      <c r="D143" t="s">
+        <v>12</v>
+      </c>
+      <c r="E143" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A143" t="s">
+      <c r="E144" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
         <v>149</v>
       </c>
-      <c r="B143" t="s">
-        <v>12</v>
-      </c>
-      <c r="C143" t="s">
-        <v>12</v>
-      </c>
-      <c r="D143" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A144" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A145" t="s">
+      <c r="B145" t="s">
+        <v>12</v>
+      </c>
+      <c r="C145" t="s">
+        <v>12</v>
+      </c>
+      <c r="D145" t="s">
+        <v>12</v>
+      </c>
+      <c r="E145" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
         <v>150</v>
       </c>
-      <c r="B145" t="s">
-        <v>12</v>
-      </c>
-      <c r="C145" t="s">
-        <v>12</v>
-      </c>
-      <c r="D145" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A146" t="s">
+      <c r="E146" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A147" t="s">
+      <c r="B147" t="s">
+        <v>12</v>
+      </c>
+      <c r="C147" t="s">
+        <v>12</v>
+      </c>
+      <c r="D147" t="s">
+        <v>12</v>
+      </c>
+      <c r="E147" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
         <v>152</v>
       </c>
-      <c r="B147" t="s">
-        <v>12</v>
-      </c>
-      <c r="C147" t="s">
-        <v>12</v>
-      </c>
-      <c r="D147" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A148" t="s">
+      <c r="E148" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A149" t="s">
+      <c r="B149" t="s">
+        <v>12</v>
+      </c>
+      <c r="C149" t="s">
+        <v>12</v>
+      </c>
+      <c r="D149" t="s">
+        <v>12</v>
+      </c>
+      <c r="E149" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A150" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="B149" t="s">
-        <v>12</v>
-      </c>
-      <c r="C149" t="s">
-        <v>12</v>
-      </c>
-      <c r="D149" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A150" s="4" t="s">
+      <c r="E150" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>156</v>
+      </c>
+      <c r="B151" t="s">
+        <v>12</v>
+      </c>
+      <c r="C151" t="s">
+        <v>12</v>
+      </c>
+      <c r="D151" t="s">
+        <v>12</v>
+      </c>
+      <c r="E151" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A151" t="s">
+      <c r="E152" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
         <v>157</v>
       </c>
-      <c r="B151" t="s">
-        <v>12</v>
-      </c>
-      <c r="C151" t="s">
-        <v>12</v>
-      </c>
-      <c r="D151" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A152" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A153" t="s">
+      <c r="B153" t="s">
+        <v>12</v>
+      </c>
+      <c r="C153" t="s">
+        <v>12</v>
+      </c>
+      <c r="D153" t="s">
+        <v>12</v>
+      </c>
+      <c r="E153" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
         <v>158</v>
       </c>
-      <c r="B153" t="s">
-        <v>12</v>
-      </c>
-      <c r="C153" t="s">
-        <v>12</v>
-      </c>
-      <c r="D153" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A154" t="s">
+      <c r="E154" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A155" t="s">
+      <c r="B155" t="s">
+        <v>12</v>
+      </c>
+      <c r="C155" t="s">
+        <v>12</v>
+      </c>
+      <c r="D155" t="s">
+        <v>12</v>
+      </c>
+      <c r="E155" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
         <v>160</v>
       </c>
-      <c r="B155" t="s">
-        <v>12</v>
-      </c>
-      <c r="C155" t="s">
-        <v>12</v>
-      </c>
-      <c r="D155" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A156" t="s">
+      <c r="E156" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A157" t="s">
+      <c r="B157" t="s">
+        <v>12</v>
+      </c>
+      <c r="C157" t="s">
+        <v>12</v>
+      </c>
+      <c r="D157" t="s">
+        <v>12</v>
+      </c>
+      <c r="E157" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
         <v>162</v>
       </c>
-      <c r="B157" t="s">
-        <v>12</v>
-      </c>
-      <c r="C157" t="s">
-        <v>12</v>
-      </c>
-      <c r="D157" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A158" t="s">
+      <c r="E158" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A159" t="s">
+      <c r="E159" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A160" t="s">
-        <v>165</v>
-      </c>
       <c r="B160" t="s">
         <v>12</v>
       </c>
@@ -2313,17 +2820,23 @@
         <v>12</v>
       </c>
       <c r="D160" t="s">
+        <v>12</v>
+      </c>
+      <c r="E160" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>166</v>
+        <v>165</v>
+      </c>
+      <c r="E161" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B162" t="s">
         <v>12</v>
@@ -2332,27 +2845,39 @@
         <v>12</v>
       </c>
       <c r="D162" t="s">
+        <v>12</v>
+      </c>
+      <c r="E162" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>168</v>
+        <v>167</v>
+      </c>
+      <c r="E163" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>169</v>
+        <v>168</v>
+      </c>
+      <c r="E164" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>170</v>
+        <v>169</v>
+      </c>
+      <c r="E165" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B166" t="s">
         <v>12</v>
@@ -2361,22 +2886,31 @@
         <v>12</v>
       </c>
       <c r="D166" t="s">
+        <v>12</v>
+      </c>
+      <c r="E166" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>172</v>
+        <v>171</v>
+      </c>
+      <c r="E167" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>191</v>
+        <v>190</v>
+      </c>
+      <c r="E168" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B169" t="s">
         <v>12</v>
@@ -2385,12 +2919,15 @@
         <v>12</v>
       </c>
       <c r="D169" t="s">
+        <v>12</v>
+      </c>
+      <c r="E169" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B170" t="s">
         <v>12</v>
@@ -2399,22 +2936,31 @@
         <v>12</v>
       </c>
       <c r="D170" t="s">
+        <v>12</v>
+      </c>
+      <c r="E170" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>175</v>
+        <v>174</v>
+      </c>
+      <c r="E171" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>176</v>
+        <v>175</v>
+      </c>
+      <c r="E172" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B173" t="s">
         <v>12</v>
@@ -2423,65 +2969,96 @@
         <v>12</v>
       </c>
       <c r="D173" t="s">
+        <v>12</v>
+      </c>
+      <c r="E173" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B174" s="3"/>
       <c r="C174" s="3"/>
       <c r="D174" s="3"/>
-      <c r="E174" s="3"/>
+      <c r="E174" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B175" s="3"/>
       <c r="C175" s="3"/>
       <c r="D175" s="3"/>
-      <c r="E175" s="3"/>
+      <c r="E175" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>180</v>
+        <v>179</v>
+      </c>
+      <c r="E176" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>181</v>
+        <v>180</v>
+      </c>
+      <c r="E177" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>182</v>
+        <v>181</v>
+      </c>
+      <c r="E178" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>183</v>
+        <v>182</v>
+      </c>
+      <c r="E179" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>184</v>
+        <v>183</v>
+      </c>
+      <c r="E180" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>185</v>
+        <v>184</v>
+      </c>
+      <c r="E181" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>186</v>
+        <v>185</v>
+      </c>
+      <c r="E182" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>187</v>
+        <v>186</v>
+      </c>
+      <c r="E183" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.2">
@@ -2491,31 +3068,38 @@
       </c>
       <c r="B184">
         <f t="shared" ref="B184:D184" si="0">COUNTA(B2:B183)</f>
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C184">
         <f t="shared" si="0"/>
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D184">
         <f t="shared" si="0"/>
-        <v>55</v>
+        <v>57</v>
+      </c>
+      <c r="E184">
+        <f t="shared" ref="E184" si="1">COUNTA(E2:E183)</f>
+        <v>182</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B185" s="2">
         <f>B184/$A184</f>
-        <v>0.30769230769230771</v>
+        <v>0.32417582417582419</v>
       </c>
       <c r="C185" s="2">
-        <f t="shared" ref="C185:D185" si="1">C184/$A184</f>
-        <v>0.30769230769230771</v>
+        <f t="shared" ref="C185:D185" si="2">C184/$A184</f>
+        <v>0.32417582417582419</v>
       </c>
       <c r="D185" s="2">
-        <f t="shared" si="1"/>
-        <v>0.30219780219780218</v>
-      </c>
-      <c r="E185" s="2"/>
+        <f t="shared" si="2"/>
+        <v>0.31318681318681318</v>
+      </c>
+      <c r="E185" s="2">
+        <f t="shared" ref="E185" si="3">E184/$A184</f>
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
working on functional programs
</commit_message>
<xml_diff>
--- a/Supported.xlsx
+++ b/Supported.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/don/go/src/github.com/navionguy/basicwasm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0420372B-C9FB-AE4B-9625-CB8E0CFFCF55}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C48BCB8-E3C4-464A-9673-6533048D97D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19000" xr2:uid="{AA62892B-5570-A74D-BDA8-A103E896D107}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="195">
   <si>
     <t>Functions, Commands &amp; Statement</t>
   </si>
@@ -1015,10 +1015,10 @@
   <dimension ref="A1:F185"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="17280" ySplit="1800" topLeftCell="M1" activePane="bottomLeft"/>
+      <pane xSplit="17280" ySplit="1800" topLeftCell="M84" activePane="bottomLeft"/>
       <selection activeCell="E1" sqref="E1"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="H172" sqref="H172"/>
+      <selection pane="bottomLeft" activeCell="B79" sqref="B79"/>
       <selection pane="bottomRight" activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
@@ -1256,6 +1256,12 @@
       <c r="A16" t="s">
         <v>20</v>
       </c>
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
       <c r="E16" t="s">
         <v>12</v>
       </c>
@@ -1292,6 +1298,12 @@
       <c r="A19" s="4" t="s">
         <v>24</v>
       </c>
+      <c r="B19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" t="s">
+        <v>12</v>
+      </c>
       <c r="E19" t="s">
         <v>12</v>
       </c>
@@ -1308,6 +1320,9 @@
       <c r="A21" s="4" t="s">
         <v>26</v>
       </c>
+      <c r="B21" t="s">
+        <v>12</v>
+      </c>
       <c r="E21" t="s">
         <v>12</v>
       </c>
@@ -2036,6 +2051,9 @@
       <c r="A85" s="4" t="s">
         <v>90</v>
       </c>
+      <c r="B85" t="s">
+        <v>12</v>
+      </c>
       <c r="E85" t="s">
         <v>12</v>
       </c>
@@ -2223,6 +2241,9 @@
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>106</v>
+      </c>
+      <c r="B101" t="s">
+        <v>12</v>
       </c>
       <c r="E101" t="s">
         <v>12</v>
@@ -3068,11 +3089,11 @@
       </c>
       <c r="B184">
         <f t="shared" ref="B184:D184" si="0">COUNTA(B2:B183)</f>
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C184">
         <f t="shared" si="0"/>
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D184">
         <f t="shared" si="0"/>
@@ -3086,11 +3107,11 @@
     <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B185" s="2">
         <f>B184/$A184</f>
-        <v>0.32417582417582419</v>
+        <v>0.35164835164835168</v>
       </c>
       <c r="C185" s="2">
         <f t="shared" ref="C185:D185" si="2">C184/$A184</f>
-        <v>0.32417582417582419</v>
+        <v>0.33516483516483514</v>
       </c>
       <c r="D185" s="2">
         <f t="shared" si="2"/>

</xml_diff>

<commit_message>
moved builtins so parser can reference them, implemented A(5) notation for arrays
</commit_message>
<xml_diff>
--- a/Supported.xlsx
+++ b/Supported.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/don/go/src/github.com/navionguy/basicwasm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C48BCB8-E3C4-464A-9673-6533048D97D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F96F7F56-A789-6640-BBAB-E26C3184F7D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19000" xr2:uid="{AA62892B-5570-A74D-BDA8-A103E896D107}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="193">
   <si>
     <t>Functions, Commands &amp; Statement</t>
   </si>
@@ -419,6 +420,9 @@
     <t>PLAY</t>
   </si>
   <si>
+    <t>PLAN()</t>
+  </si>
+  <si>
     <t>PMAP</t>
   </si>
   <si>
@@ -609,15 +613,6 @@
   </si>
   <si>
     <t>Token File</t>
-  </si>
-  <si>
-    <t>options</t>
-  </si>
-  <si>
-    <t>spelled out</t>
-  </si>
-  <si>
-    <t>PLAY()</t>
   </si>
 </sst>
 </file>
@@ -1015,10 +1010,10 @@
   <dimension ref="A1:F185"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="17280" ySplit="1800" topLeftCell="M84" activePane="bottomLeft"/>
+      <pane xSplit="17280" ySplit="1800" topLeftCell="M1" activePane="bottomLeft"/>
       <selection activeCell="E1" sqref="E1"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="B79" sqref="B79"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
       <selection pane="bottomRight" activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
@@ -1041,7 +1036,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -1060,9 +1055,6 @@
       <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -1077,9 +1069,6 @@
       <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -1094,9 +1083,6 @@
       <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -1111,9 +1097,6 @@
       <c r="D5" t="s">
         <v>12</v>
       </c>
-      <c r="E5" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -1128,9 +1111,6 @@
       <c r="D6" t="s">
         <v>12</v>
       </c>
-      <c r="E6" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -1139,9 +1119,7 @@
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
-      <c r="E7" t="s">
-        <v>12</v>
-      </c>
+      <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -1150,9 +1128,7 @@
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
-      <c r="E8" t="s">
-        <v>12</v>
-      </c>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -1161,9 +1137,7 @@
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
-      <c r="E9" t="s">
-        <v>12</v>
-      </c>
+      <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -1178,9 +1152,6 @@
       <c r="D10" t="s">
         <v>12</v>
       </c>
-      <c r="E10" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
@@ -1192,23 +1163,11 @@
       <c r="C11" t="s">
         <v>12</v>
       </c>
-      <c r="D11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" t="s">
-        <v>192</v>
-      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
-      <c r="E12" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -1223,9 +1182,6 @@
       <c r="D13" t="s">
         <v>12</v>
       </c>
-      <c r="E13" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -1240,39 +1196,21 @@
       <c r="D14" t="s">
         <v>12</v>
       </c>
-      <c r="E14" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>19</v>
       </c>
-      <c r="E15" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>20</v>
       </c>
-      <c r="B16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>21</v>
       </c>
-      <c r="E17" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
@@ -1287,9 +1225,6 @@
       <c r="D18" t="s">
         <v>12</v>
       </c>
-      <c r="E18" t="s">
-        <v>12</v>
-      </c>
       <c r="F18" t="s">
         <v>23</v>
       </c>
@@ -1304,17 +1239,11 @@
       <c r="C19" t="s">
         <v>12</v>
       </c>
-      <c r="E19" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>25</v>
       </c>
-      <c r="E20" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
@@ -1323,7 +1252,7 @@
       <c r="B21" t="s">
         <v>12</v>
       </c>
-      <c r="E21" t="s">
+      <c r="C21" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1331,9 +1260,6 @@
       <c r="A22" t="s">
         <v>27</v>
       </c>
-      <c r="E22" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
@@ -1348,9 +1274,6 @@
       <c r="D23" t="s">
         <v>12</v>
       </c>
-      <c r="E23" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
@@ -1365,23 +1288,11 @@
       <c r="D24" t="s">
         <v>12</v>
       </c>
-      <c r="E24" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B25" t="s">
-        <v>12</v>
-      </c>
-      <c r="C25" t="s">
-        <v>12</v>
-      </c>
-      <c r="E25" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
@@ -1396,9 +1307,6 @@
       <c r="D26" t="s">
         <v>12</v>
       </c>
-      <c r="E26" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
@@ -1413,9 +1321,6 @@
       <c r="D27" t="s">
         <v>12</v>
       </c>
-      <c r="E27" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
@@ -1430,9 +1335,6 @@
       <c r="D28" t="s">
         <v>12</v>
       </c>
-      <c r="E28" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
@@ -1447,17 +1349,11 @@
       <c r="D29" t="s">
         <v>12</v>
       </c>
-      <c r="E29" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>35</v>
       </c>
-      <c r="E30" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
@@ -1472,70 +1368,43 @@
       <c r="D31" t="s">
         <v>12</v>
       </c>
-      <c r="E31" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>37</v>
       </c>
-      <c r="E32" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>38</v>
       </c>
-      <c r="E33" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>39</v>
       </c>
-      <c r="E34" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>40</v>
       </c>
-      <c r="E35" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>41</v>
       </c>
-      <c r="E36" t="s">
-        <v>12</v>
-      </c>
-      <c r="F36" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>42</v>
       </c>
-      <c r="E37" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>43</v>
       </c>
-      <c r="E38" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>44</v>
       </c>
@@ -1548,27 +1417,18 @@
       <c r="D39" t="s">
         <v>12</v>
       </c>
-      <c r="E39" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>45</v>
       </c>
-      <c r="E40" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>46</v>
       </c>
-      <c r="E41" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>47</v>
       </c>
@@ -1581,73 +1441,46 @@
       <c r="D42" t="s">
         <v>12</v>
       </c>
-      <c r="E42" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>48</v>
       </c>
-      <c r="E43" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>49</v>
       </c>
-      <c r="E44" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>50</v>
       </c>
-      <c r="E45" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>51</v>
       </c>
-      <c r="E46" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>52</v>
       </c>
-      <c r="E47" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>53</v>
-      </c>
-      <c r="E48" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>54</v>
       </c>
-      <c r="E49" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>55</v>
       </c>
-      <c r="E50" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
@@ -1662,25 +1495,16 @@
       <c r="D51" t="s">
         <v>12</v>
       </c>
-      <c r="E51" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>57</v>
       </c>
-      <c r="E52" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>58</v>
       </c>
-      <c r="E53" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
@@ -1695,9 +1519,6 @@
       <c r="D54" t="s">
         <v>12</v>
       </c>
-      <c r="E54" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
@@ -1712,33 +1533,21 @@
       <c r="D55" t="s">
         <v>12</v>
       </c>
-      <c r="E55" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>61</v>
       </c>
-      <c r="E56" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>62</v>
       </c>
-      <c r="E57" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>63</v>
       </c>
-      <c r="E58" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
@@ -1750,9 +1559,6 @@
       <c r="C59" t="s">
         <v>12</v>
       </c>
-      <c r="E59" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
@@ -1767,9 +1573,6 @@
       <c r="D60" t="s">
         <v>12</v>
       </c>
-      <c r="E60" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
@@ -1784,9 +1587,6 @@
       <c r="D61" t="s">
         <v>12</v>
       </c>
-      <c r="E61" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
@@ -1801,9 +1601,6 @@
       <c r="D62" t="s">
         <v>12</v>
       </c>
-      <c r="E62" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
@@ -1818,46 +1615,31 @@
       <c r="D63" t="s">
         <v>12</v>
       </c>
-      <c r="E63" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>69</v>
       </c>
-      <c r="E64" t="s">
-        <v>12</v>
-      </c>
       <c r="F64" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>70</v>
       </c>
-      <c r="E65" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>71</v>
       </c>
-      <c r="E66" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>72</v>
       </c>
-      <c r="E67" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>73</v>
       </c>
@@ -1870,11 +1652,8 @@
       <c r="D68" t="s">
         <v>12</v>
       </c>
-      <c r="E68" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>74</v>
       </c>
@@ -1887,51 +1666,33 @@
       <c r="D69" t="s">
         <v>12</v>
       </c>
-      <c r="E69" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>75</v>
       </c>
-      <c r="E70" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>76</v>
       </c>
-      <c r="E71" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="E72" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>78</v>
       </c>
-      <c r="E73" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>79</v>
       </c>
-      <c r="E74" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>80</v>
       </c>
@@ -1944,11 +1705,8 @@
       <c r="D75" t="s">
         <v>12</v>
       </c>
-      <c r="E75" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>81</v>
       </c>
@@ -1961,11 +1719,8 @@
       <c r="D76" t="s">
         <v>12</v>
       </c>
-      <c r="E76" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>82</v>
       </c>
@@ -1978,32 +1733,20 @@
       <c r="D77" t="s">
         <v>12</v>
       </c>
-      <c r="E77" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>83</v>
       </c>
-      <c r="E78" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>84</v>
       </c>
-      <c r="E79" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>85</v>
-      </c>
-      <c r="E80" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
@@ -2019,33 +1762,21 @@
       <c r="D81" t="s">
         <v>12</v>
       </c>
-      <c r="E81" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>87</v>
       </c>
-      <c r="E82" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>88</v>
       </c>
-      <c r="E83" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>89</v>
       </c>
-      <c r="E84" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
@@ -2054,7 +1785,7 @@
       <c r="B85" t="s">
         <v>12</v>
       </c>
-      <c r="E85" t="s">
+      <c r="C85" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2062,17 +1793,11 @@
       <c r="A86" t="s">
         <v>91</v>
       </c>
-      <c r="E86" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>92</v>
       </c>
-      <c r="E87" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
@@ -2087,9 +1812,6 @@
       <c r="D88" t="s">
         <v>12</v>
       </c>
-      <c r="E88" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
@@ -2104,44 +1826,29 @@
       <c r="D89" t="s">
         <v>12</v>
       </c>
-      <c r="E89" t="s">
-        <v>12</v>
-      </c>
       <c r="F89" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>95</v>
       </c>
-      <c r="E90" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>96</v>
       </c>
-      <c r="E91" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>97</v>
       </c>
-      <c r="E92" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>98</v>
       </c>
-      <c r="E93" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
@@ -2156,20 +1863,14 @@
       <c r="D94" t="s">
         <v>12</v>
       </c>
-      <c r="E94" t="s">
-        <v>12</v>
-      </c>
       <c r="F94" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>100</v>
       </c>
-      <c r="E95" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
@@ -2184,11 +1885,8 @@
       <c r="D96" t="s">
         <v>12</v>
       </c>
-      <c r="E96" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>102</v>
       </c>
@@ -2201,11 +1899,8 @@
       <c r="D97" t="s">
         <v>12</v>
       </c>
-      <c r="E97" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>103</v>
       </c>
@@ -2218,38 +1913,23 @@
       <c r="D98" t="s">
         <v>12</v>
       </c>
-      <c r="E98" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>104</v>
       </c>
-      <c r="E99" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>105</v>
       </c>
-      <c r="E100" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>106</v>
       </c>
-      <c r="B101" t="s">
-        <v>12</v>
-      </c>
-      <c r="E101" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>107</v>
       </c>
@@ -2262,229 +1942,145 @@
       <c r="D102" t="s">
         <v>12</v>
       </c>
-      <c r="E102" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>108</v>
       </c>
-      <c r="E103" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>109</v>
       </c>
-      <c r="E104" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>110</v>
       </c>
-      <c r="E105" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>111</v>
       </c>
-      <c r="E106" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>112</v>
       </c>
-      <c r="E107" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>113</v>
       </c>
-      <c r="E108" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>114</v>
       </c>
-      <c r="E109" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>115</v>
       </c>
-      <c r="E110" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>116</v>
       </c>
-      <c r="E111" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>117</v>
       </c>
-      <c r="E112" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>118</v>
       </c>
-      <c r="E113" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>119</v>
       </c>
-      <c r="E114" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>120</v>
       </c>
-      <c r="E115" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>121</v>
       </c>
-      <c r="E116" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>122</v>
       </c>
-      <c r="E117" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>123</v>
       </c>
-      <c r="E118" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>124</v>
       </c>
-      <c r="E119" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>125</v>
       </c>
-      <c r="E120" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>126</v>
       </c>
-      <c r="E121" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>127</v>
       </c>
-      <c r="E122" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>194</v>
-      </c>
-      <c r="E123" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>128</v>
-      </c>
-      <c r="E124" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>129</v>
-      </c>
-      <c r="E125" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>130</v>
-      </c>
-      <c r="E126" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>131</v>
-      </c>
-      <c r="E127" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>132</v>
-      </c>
-      <c r="E128" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>133</v>
-      </c>
-      <c r="E129" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B130" t="s">
         <v>12</v>
@@ -2495,53 +2091,35 @@
       <c r="D130" t="s">
         <v>12</v>
       </c>
-      <c r="E130" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>135</v>
-      </c>
-      <c r="E131" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>136</v>
-      </c>
-      <c r="E132" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>137</v>
-      </c>
-      <c r="E133" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>138</v>
-      </c>
-      <c r="E134" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>139</v>
-      </c>
-      <c r="E135" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B136" t="s">
         <v>12</v>
@@ -2552,13 +2130,10 @@
       <c r="D136" t="s">
         <v>12</v>
       </c>
-      <c r="E136" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B137" t="s">
         <v>12</v>
@@ -2569,29 +2144,20 @@
       <c r="D137" t="s">
         <v>12</v>
       </c>
-      <c r="E137" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>142</v>
-      </c>
-      <c r="E138" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>143</v>
-      </c>
-      <c r="E139" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B140" t="s">
         <v>12</v>
@@ -2602,54 +2168,39 @@
       <c r="D140" t="s">
         <v>12</v>
       </c>
-      <c r="E140" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>145</v>
-      </c>
-      <c r="E141" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>146</v>
-      </c>
-      <c r="E142" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
+        <v>149</v>
+      </c>
+      <c r="B143" t="s">
+        <v>12</v>
+      </c>
+      <c r="C143" t="s">
+        <v>12</v>
+      </c>
+      <c r="D143" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
         <v>148</v>
       </c>
-      <c r="B143" t="s">
-        <v>12</v>
-      </c>
-      <c r="C143" t="s">
-        <v>12</v>
-      </c>
-      <c r="D143" t="s">
-        <v>12</v>
-      </c>
-      <c r="E143" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A144" t="s">
-        <v>147</v>
-      </c>
-      <c r="E144" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B145" t="s">
         <v>12</v>
@@ -2660,21 +2211,15 @@
       <c r="D145" t="s">
         <v>12</v>
       </c>
-      <c r="E145" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>150</v>
-      </c>
-      <c r="E146" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B147" t="s">
         <v>12</v>
@@ -2685,21 +2230,15 @@
       <c r="D147" t="s">
         <v>12</v>
       </c>
-      <c r="E147" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>152</v>
-      </c>
-      <c r="E148" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B149" t="s">
         <v>12</v>
@@ -2710,46 +2249,34 @@
       <c r="D149" t="s">
         <v>12</v>
       </c>
-      <c r="E149" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="E150" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
+        <v>157</v>
+      </c>
+      <c r="B151" t="s">
+        <v>12</v>
+      </c>
+      <c r="C151" t="s">
+        <v>12</v>
+      </c>
+      <c r="D151" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
         <v>156</v>
       </c>
-      <c r="B151" t="s">
-        <v>12</v>
-      </c>
-      <c r="C151" t="s">
-        <v>12</v>
-      </c>
-      <c r="D151" t="s">
-        <v>12</v>
-      </c>
-      <c r="E151" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A152" t="s">
-        <v>155</v>
-      </c>
-      <c r="E152" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B153" t="s">
         <v>12</v>
@@ -2760,21 +2287,15 @@
       <c r="D153" t="s">
         <v>12</v>
       </c>
-      <c r="E153" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>158</v>
-      </c>
-      <c r="E154" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B155" t="s">
         <v>12</v>
@@ -2785,21 +2306,15 @@
       <c r="D155" t="s">
         <v>12</v>
       </c>
-      <c r="E155" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>160</v>
-      </c>
-      <c r="E156" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B157" t="s">
         <v>12</v>
@@ -2810,29 +2325,20 @@
       <c r="D157" t="s">
         <v>12</v>
       </c>
-      <c r="E157" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>162</v>
-      </c>
-      <c r="E158" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>163</v>
-      </c>
-      <c r="E159" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B160" t="s">
         <v>12</v>
@@ -2841,23 +2347,17 @@
         <v>12</v>
       </c>
       <c r="D160" t="s">
-        <v>12</v>
-      </c>
-      <c r="E160" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>165</v>
-      </c>
-      <c r="E161" t="s">
-        <v>12</v>
+        <v>166</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B162" t="s">
         <v>12</v>
@@ -2866,39 +2366,27 @@
         <v>12</v>
       </c>
       <c r="D162" t="s">
-        <v>12</v>
-      </c>
-      <c r="E162" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>167</v>
-      </c>
-      <c r="E163" t="s">
-        <v>12</v>
+        <v>168</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>168</v>
-      </c>
-      <c r="E164" t="s">
-        <v>12</v>
+        <v>169</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>169</v>
-      </c>
-      <c r="E165" t="s">
-        <v>12</v>
+        <v>170</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B166" t="s">
         <v>12</v>
@@ -2907,31 +2395,22 @@
         <v>12</v>
       </c>
       <c r="D166" t="s">
-        <v>12</v>
-      </c>
-      <c r="E166" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>171</v>
-      </c>
-      <c r="E167" t="s">
-        <v>12</v>
+        <v>172</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>190</v>
-      </c>
-      <c r="E168" t="s">
-        <v>12</v>
+        <v>191</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B169" t="s">
         <v>12</v>
@@ -2940,15 +2419,12 @@
         <v>12</v>
       </c>
       <c r="D169" t="s">
-        <v>12</v>
-      </c>
-      <c r="E169" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B170" t="s">
         <v>12</v>
@@ -2957,31 +2433,22 @@
         <v>12</v>
       </c>
       <c r="D170" t="s">
-        <v>12</v>
-      </c>
-      <c r="E170" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>174</v>
-      </c>
-      <c r="E171" t="s">
-        <v>12</v>
+        <v>175</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>175</v>
-      </c>
-      <c r="E172" t="s">
-        <v>12</v>
+        <v>176</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B173" t="s">
         <v>12</v>
@@ -2990,96 +2457,65 @@
         <v>12</v>
       </c>
       <c r="D173" t="s">
-        <v>12</v>
-      </c>
-      <c r="E173" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B174" s="3"/>
       <c r="C174" s="3"/>
       <c r="D174" s="3"/>
-      <c r="E174" t="s">
-        <v>12</v>
-      </c>
+      <c r="E174" s="3"/>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B175" s="3"/>
       <c r="C175" s="3"/>
       <c r="D175" s="3"/>
-      <c r="E175" t="s">
-        <v>12</v>
-      </c>
+      <c r="E175" s="3"/>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>179</v>
-      </c>
-      <c r="E176" t="s">
-        <v>12</v>
+        <v>180</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>180</v>
-      </c>
-      <c r="E177" t="s">
-        <v>12</v>
+        <v>181</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>181</v>
-      </c>
-      <c r="E178" t="s">
-        <v>12</v>
+        <v>182</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>182</v>
-      </c>
-      <c r="E179" t="s">
-        <v>12</v>
+        <v>183</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>183</v>
-      </c>
-      <c r="E180" t="s">
-        <v>12</v>
+        <v>184</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>184</v>
-      </c>
-      <c r="E181" t="s">
-        <v>12</v>
+        <v>185</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>185</v>
-      </c>
-      <c r="E182" t="s">
-        <v>12</v>
+        <v>186</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>186</v>
-      </c>
-      <c r="E183" t="s">
-        <v>12</v>
+        <v>187</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.2">
@@ -3088,39 +2524,32 @@
         <v>182</v>
       </c>
       <c r="B184">
-        <f t="shared" ref="B184:D184" si="0">COUNTA(B2:B183)</f>
-        <v>64</v>
+        <f>COUNTA(B2:B183)</f>
+        <v>61</v>
       </c>
       <c r="C184">
-        <f t="shared" si="0"/>
+        <f>COUNTA(C2:C183)</f>
         <v>61</v>
       </c>
       <c r="D184">
-        <f t="shared" si="0"/>
-        <v>57</v>
-      </c>
-      <c r="E184">
-        <f t="shared" ref="E184" si="1">COUNTA(E2:E183)</f>
-        <v>182</v>
+        <f>COUNTA(D2:D183)</f>
+        <v>56</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B185" s="2">
         <f>B184/$A184</f>
-        <v>0.35164835164835168</v>
+        <v>0.33516483516483514</v>
       </c>
       <c r="C185" s="2">
-        <f t="shared" ref="C185:D185" si="2">C184/$A184</f>
+        <f>C184/$A184</f>
         <v>0.33516483516483514</v>
       </c>
       <c r="D185" s="2">
-        <f t="shared" si="2"/>
-        <v>0.31318681318681318</v>
-      </c>
-      <c r="E185" s="2">
-        <f t="shared" ref="E185" si="3">E184/$A184</f>
-        <v>1</v>
-      </c>
+        <f>D184/$A184</f>
+        <v>0.30769230769230771</v>
+      </c>
+      <c r="E185" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Working on adding screen control statemnts, more code coverage, settings storage
</commit_message>
<xml_diff>
--- a/Supported.xlsx
+++ b/Supported.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/don/go/src/github.com/navionguy/basicwasm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F96F7F56-A789-6640-BBAB-E26C3184F7D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A17797-B5B4-3947-8A02-14707383B3EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19000" xr2:uid="{AA62892B-5570-A74D-BDA8-A103E896D107}"/>
+    <workbookView xWindow="1220" yWindow="2000" windowWidth="33600" windowHeight="19000" xr2:uid="{AA62892B-5570-A74D-BDA8-A103E896D107}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +26,7 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="196">
   <si>
     <t>Functions, Commands &amp; Statement</t>
   </si>
@@ -613,13 +613,22 @@
   </si>
   <si>
     <t>Token File</t>
+  </si>
+  <si>
+    <t>Builtins</t>
+  </si>
+  <si>
+    <t>Bare minimum</t>
+  </si>
+  <si>
+    <t>b</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -644,6 +653,13 @@
     <font>
       <sz val="12"/>
       <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -682,7 +698,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -690,6 +706,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1007,46 +1024,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{264AD530-8319-C14F-BA84-D94176E8A777}">
-  <dimension ref="A1:F185"/>
+  <dimension ref="A1:G185"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="17280" ySplit="1800" topLeftCell="M1" activePane="bottomLeft"/>
-      <selection activeCell="E1" sqref="E1"/>
+      <pane xSplit="17280" ySplit="1800" topLeftCell="M110" activePane="bottomLeft"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomLeft" activeCell="D118" sqref="D118"/>
       <selection pane="bottomRight" activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>192</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C2" t="s">
@@ -1055,12 +1075,15 @@
       <c r="D2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C3" t="s">
@@ -1069,12 +1092,15 @@
       <c r="D3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C4" t="s">
@@ -1083,36 +1109,39 @@
       <c r="D4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
       <c r="C5" t="s">
         <v>12</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
       <c r="C6" t="s">
         <v>12</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1120,8 +1149,9 @@
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1129,8 +1159,9 @@
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1138,8 +1169,9 @@
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1152,24 +1184,31 @@
       <c r="D10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B11" t="s">
-        <v>12</v>
-      </c>
+      <c r="B11" s="4"/>
       <c r="C11" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1182,8 +1221,11 @@
       <c r="D13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1196,72 +1238,95 @@
       <c r="D14" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>22</v>
       </c>
-      <c r="B18" t="s">
-        <v>12</v>
-      </c>
       <c r="C18" t="s">
         <v>12</v>
       </c>
       <c r="D18" t="s">
         <v>12</v>
       </c>
-      <c r="F18" t="s">
+      <c r="E18" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B19" t="s">
-        <v>12</v>
-      </c>
+      <c r="B19" s="4"/>
       <c r="C19" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B21" t="s">
-        <v>12</v>
-      </c>
+      <c r="B21" s="4"/>
       <c r="C21" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -1274,8 +1339,11 @@
       <c r="D23" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -1288,13 +1356,26 @@
       <c r="D24" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B25" s="4"/>
+      <c r="C25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -1307,8 +1388,11 @@
       <c r="D26" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -1321,8 +1405,11 @@
       <c r="D27" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -1335,192 +1422,195 @@
       <c r="D28" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E28" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>34</v>
       </c>
-      <c r="B29" t="s">
-        <v>12</v>
-      </c>
       <c r="C29" t="s">
         <v>12</v>
       </c>
       <c r="D29" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E29" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>36</v>
       </c>
-      <c r="B31" t="s">
-        <v>12</v>
-      </c>
       <c r="C31" t="s">
         <v>12</v>
       </c>
       <c r="D31" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E31" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>44</v>
       </c>
-      <c r="B39" t="s">
-        <v>12</v>
-      </c>
       <c r="C39" t="s">
         <v>12</v>
       </c>
       <c r="D39" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E39" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>47</v>
       </c>
-      <c r="B42" t="s">
-        <v>12</v>
-      </c>
       <c r="C42" t="s">
         <v>12</v>
       </c>
       <c r="D42" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E42" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>56</v>
       </c>
-      <c r="B51" t="s">
-        <v>12</v>
-      </c>
       <c r="C51" t="s">
         <v>12</v>
       </c>
       <c r="D51" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E51" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>59</v>
       </c>
-      <c r="B54" t="s">
-        <v>12</v>
-      </c>
       <c r="C54" t="s">
         <v>12</v>
       </c>
       <c r="D54" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E54" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>60</v>
       </c>
@@ -1533,48 +1623,55 @@
       <c r="D55" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E55" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B59" t="s">
-        <v>12</v>
-      </c>
+      <c r="B59" s="4"/>
       <c r="C59" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D59" t="s">
+        <v>12</v>
+      </c>
+      <c r="E59" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>65</v>
       </c>
-      <c r="B60" t="s">
-        <v>12</v>
-      </c>
       <c r="C60" t="s">
         <v>12</v>
       </c>
       <c r="D60" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E60" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>66</v>
       </c>
@@ -1587,59 +1684,62 @@
       <c r="D61" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E61" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>67</v>
       </c>
-      <c r="B62" t="s">
-        <v>12</v>
-      </c>
       <c r="C62" t="s">
         <v>12</v>
       </c>
       <c r="D62" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E62" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>68</v>
       </c>
-      <c r="B63" t="s">
-        <v>12</v>
-      </c>
       <c r="C63" t="s">
         <v>12</v>
       </c>
       <c r="D63" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E63" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>69</v>
       </c>
-      <c r="F64" t="s">
+      <c r="G64" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>73</v>
       </c>
@@ -1652,8 +1752,11 @@
       <c r="D68" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E68" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>74</v>
       </c>
@@ -1666,33 +1769,37 @@
       <c r="D69" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E69" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B72" s="4"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>80</v>
       </c>
@@ -1705,8 +1812,11 @@
       <c r="D75" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E75" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>81</v>
       </c>
@@ -1719,87 +1829,100 @@
       <c r="D76" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E76" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>82</v>
       </c>
-      <c r="B77" t="s">
-        <v>12</v>
-      </c>
       <c r="C77" t="s">
         <v>12</v>
       </c>
       <c r="D77" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E77" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>86</v>
       </c>
-      <c r="B81" t="s">
-        <v>12</v>
-      </c>
       <c r="C81" t="s">
         <v>12</v>
       </c>
       <c r="D81" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E81" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C83" t="s">
+        <v>12</v>
+      </c>
+      <c r="D83" t="s">
+        <v>12</v>
+      </c>
+      <c r="E83" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B85" t="s">
-        <v>12</v>
-      </c>
+      <c r="B85" s="4"/>
       <c r="C85" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D85" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>93</v>
       </c>
@@ -1812,8 +1935,11 @@
       <c r="D88" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E88" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>94</v>
       </c>
@@ -1826,31 +1952,34 @@
       <c r="D89" t="s">
         <v>12</v>
       </c>
-      <c r="F89" t="s">
+      <c r="E89" t="s">
+        <v>12</v>
+      </c>
+      <c r="G89" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>99</v>
       </c>
@@ -1863,16 +1992,19 @@
       <c r="D94" t="s">
         <v>12</v>
       </c>
-      <c r="F94" t="s">
+      <c r="E94" t="s">
+        <v>12</v>
+      </c>
+      <c r="G94" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>101</v>
       </c>
@@ -1885,8 +2017,11 @@
       <c r="D96" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E96" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>102</v>
       </c>
@@ -1899,8 +2034,11 @@
       <c r="D97" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E97" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>103</v>
       </c>
@@ -1913,23 +2051,35 @@
       <c r="D98" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E98" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C101" t="s">
+        <v>12</v>
+      </c>
+      <c r="D101" t="s">
+        <v>12</v>
+      </c>
+      <c r="E101" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>107</v>
       </c>
@@ -1942,244 +2092,265 @@
       <c r="D102" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E102" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C117" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C118" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>135</v>
       </c>
-      <c r="B130" t="s">
-        <v>12</v>
-      </c>
       <c r="C130" t="s">
         <v>12</v>
       </c>
       <c r="D130" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E130" t="s">
+        <v>195</v>
+      </c>
+      <c r="G130" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>141</v>
       </c>
-      <c r="B136" t="s">
-        <v>12</v>
-      </c>
       <c r="C136" t="s">
         <v>12</v>
       </c>
       <c r="D136" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E136" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>142</v>
       </c>
-      <c r="B137" t="s">
-        <v>12</v>
-      </c>
       <c r="C137" t="s">
         <v>12</v>
       </c>
       <c r="D137" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E137" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>145</v>
       </c>
-      <c r="B140" t="s">
-        <v>12</v>
-      </c>
       <c r="C140" t="s">
         <v>12</v>
       </c>
       <c r="D140" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E140" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C142" t="s">
+        <v>12</v>
+      </c>
+      <c r="D142" t="s">
+        <v>12</v>
+      </c>
+      <c r="E142" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>149</v>
       </c>
@@ -2192,51 +2363,54 @@
       <c r="D143" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E143" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>150</v>
       </c>
-      <c r="B145" t="s">
-        <v>12</v>
-      </c>
       <c r="C145" t="s">
         <v>12</v>
       </c>
       <c r="D145" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E145" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>152</v>
       </c>
-      <c r="B147" t="s">
-        <v>12</v>
-      </c>
       <c r="C147" t="s">
         <v>12</v>
       </c>
       <c r="D147" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E147" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>154</v>
       </c>
@@ -2249,13 +2423,26 @@
       <c r="D149" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E149" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150" s="4" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B150" s="4"/>
+      <c r="C150" t="s">
+        <v>12</v>
+      </c>
+      <c r="D150" t="s">
+        <v>12</v>
+      </c>
+      <c r="E150" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>157</v>
       </c>
@@ -2268,13 +2455,16 @@
       <c r="D151" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E151" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>158</v>
       </c>
@@ -2287,13 +2477,16 @@
       <c r="D153" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E153" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>160</v>
       </c>
@@ -2306,13 +2499,16 @@
       <c r="D155" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E155" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>162</v>
       </c>
@@ -2325,18 +2521,30 @@
       <c r="D157" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E157" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C159" t="s">
+        <v>12</v>
+      </c>
+      <c r="D159" t="s">
+        <v>12</v>
+      </c>
+      <c r="E159" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>165</v>
       </c>
@@ -2349,13 +2557,16 @@
       <c r="D160" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E160" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>167</v>
       </c>
@@ -2368,23 +2579,26 @@
       <c r="D162" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E162" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>171</v>
       </c>
@@ -2397,56 +2611,59 @@
       <c r="D166" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E166" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>173</v>
       </c>
-      <c r="B169" t="s">
-        <v>12</v>
-      </c>
       <c r="C169" t="s">
         <v>12</v>
       </c>
       <c r="D169" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E169" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>174</v>
       </c>
-      <c r="B170" t="s">
-        <v>12</v>
-      </c>
       <c r="C170" t="s">
         <v>12</v>
       </c>
       <c r="D170" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E170" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>177</v>
       </c>
@@ -2459,97 +2676,108 @@
       <c r="D173" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E173" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>178</v>
       </c>
-      <c r="B174" s="3"/>
       <c r="C174" s="3"/>
       <c r="D174" s="3"/>
       <c r="E174" s="3"/>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F174" s="3"/>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>179</v>
       </c>
-      <c r="B175" s="3"/>
       <c r="C175" s="3"/>
       <c r="D175" s="3"/>
       <c r="E175" s="3"/>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F175" s="3"/>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A184">
         <f>COUNTA(A2:A183)</f>
         <v>182</v>
       </c>
       <c r="B184">
         <f>COUNTA(B2:B183)</f>
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="C184">
         <f>COUNTA(C2:C183)</f>
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="D184">
         <f>COUNTA(D2:D183)</f>
-        <v>56</v>
-      </c>
-    </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+      <c r="E184">
+        <f>COUNTA(E2:E183)</f>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B185" s="2">
         <f>B184/$A184</f>
-        <v>0.33516483516483514</v>
+        <v>0.18681318681318682</v>
       </c>
       <c r="C185" s="2">
         <f>C184/$A184</f>
-        <v>0.33516483516483514</v>
+        <v>0.39010989010989011</v>
       </c>
       <c r="D185" s="2">
         <f>D184/$A184</f>
-        <v>0.30769230769230771</v>
-      </c>
-      <c r="E185" s="2"/>
+        <v>0.37912087912087911</v>
+      </c>
+      <c r="E185" s="2">
+        <f>E184/$A184</f>
+        <v>0.36263736263736263</v>
+      </c>
+      <c r="F185" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
unit test love for cli
</commit_message>
<xml_diff>
--- a/Supported.xlsx
+++ b/Supported.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/don/go/src/github.com/navionguy/basicwasm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A17797-B5B4-3947-8A02-14707383B3EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55DA2A1C-2D56-704D-84F9-FDC7326F9A0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1220" yWindow="2000" windowWidth="33600" windowHeight="19000" xr2:uid="{AA62892B-5570-A74D-BDA8-A103E896D107}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19000" xr2:uid="{AA62892B-5570-A74D-BDA8-A103E896D107}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="196">
   <si>
     <t>Functions, Commands &amp; Statement</t>
   </si>
@@ -1027,10 +1027,10 @@
   <dimension ref="A1:G185"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="17280" ySplit="1800" topLeftCell="M110" activePane="bottomLeft"/>
+      <pane xSplit="17280" ySplit="1800" topLeftCell="M16" activePane="bottomLeft"/>
       <selection activeCell="B1" sqref="B1:B1048576"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="D118" sqref="D118"/>
+      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
       <selection pane="bottomRight" activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
@@ -1294,6 +1294,9 @@
       <c r="D19" t="s">
         <v>12</v>
       </c>
+      <c r="E19" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
@@ -2146,27 +2149,27 @@
         <v>117</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>122</v>
       </c>
@@ -2174,60 +2177,63 @@
         <v>12</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>123</v>
       </c>
       <c r="C118" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D118" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>133</v>
       </c>
@@ -2753,11 +2759,11 @@
       </c>
       <c r="D184">
         <f>COUNTA(D2:D183)</f>
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E184">
         <f>COUNTA(E2:E183)</f>
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.2">
@@ -2771,11 +2777,11 @@
       </c>
       <c r="D185" s="2">
         <f>D184/$A184</f>
-        <v>0.37912087912087911</v>
+        <v>0.38461538461538464</v>
       </c>
       <c r="E185" s="2">
         <f>E184/$A184</f>
-        <v>0.36263736263736263</v>
+        <v>0.36813186813186816</v>
       </c>
       <c r="F185" s="2"/>
     </row>

</xml_diff>

<commit_message>
LOCATE is working, ast unit testing love
</commit_message>
<xml_diff>
--- a/Supported.xlsx
+++ b/Supported.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/don/go/src/github.com/navionguy/basicwasm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55DA2A1C-2D56-704D-84F9-FDC7326F9A0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{242518E4-F5A7-6D4D-85AA-0F989C0C120A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19000" xr2:uid="{AA62892B-5570-A74D-BDA8-A103E896D107}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="197">
   <si>
     <t>Functions, Commands &amp; Statement</t>
   </si>
@@ -622,6 +622,9 @@
   </si>
   <si>
     <t>b</t>
+  </si>
+  <si>
+    <t>cursor location only</t>
   </si>
 </sst>
 </file>
@@ -1027,10 +1030,10 @@
   <dimension ref="A1:G185"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="17280" ySplit="1800" topLeftCell="M16" activePane="bottomLeft"/>
+      <pane xSplit="17280" ySplit="1800" topLeftCell="M82" activePane="bottomLeft"/>
       <selection activeCell="B1" sqref="B1:B1048576"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
+      <selection pane="bottomLeft" activeCell="G85" sqref="G85"/>
       <selection pane="bottomRight" activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
@@ -1631,9 +1634,10 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+      <c r="A56" s="4" t="s">
         <v>61</v>
       </c>
+      <c r="B56" s="4"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
@@ -1914,6 +1918,12 @@
       <c r="D85" t="s">
         <v>12</v>
       </c>
+      <c r="E85" t="s">
+        <v>12</v>
+      </c>
+      <c r="G85" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
@@ -2064,9 +2074,10 @@
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A100" t="s">
+      <c r="A100" s="4" t="s">
         <v>105</v>
       </c>
+      <c r="B100" s="4"/>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
@@ -2763,7 +2774,7 @@
       </c>
       <c r="E184">
         <f>COUNTA(E2:E183)</f>
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.2">
@@ -2781,7 +2792,7 @@
       </c>
       <c r="E185" s="2">
         <f>E184/$A184</f>
-        <v>0.36813186813186816</v>
+        <v>0.37362637362637363</v>
       </c>
       <c r="F185" s="2"/>
     </row>

</xml_diff>

<commit_message>
Implementing the VIEW PRINT statement
</commit_message>
<xml_diff>
--- a/Supported.xlsx
+++ b/Supported.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/don/go/src/github.com/navionguy/basicwasm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB170B19-9499-8F44-A412-CFE58C65780B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FBF6FDE-3C13-BC4A-AC22-FDB49241CEC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19000" xr2:uid="{AA62892B-5570-A74D-BDA8-A103E896D107}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1030,10 +1031,10 @@
   <dimension ref="A1:L185"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="17280" ySplit="1800" topLeftCell="L161" activePane="bottomLeft"/>
+      <pane xSplit="17280" ySplit="1800" topLeftCell="L147" activePane="bottomLeft"/>
       <selection activeCell="B1" sqref="B1:B1048576"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="E100" sqref="E100"/>
+      <selection pane="bottomLeft" activeCell="E177" sqref="E177"/>
       <selection pane="bottomRight" activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
@@ -2742,9 +2743,10 @@
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A177" t="s">
+      <c r="A177" s="4" t="s">
         <v>181</v>
       </c>
+      <c r="B177" s="4"/>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A178" t="s">

</xml_diff>

<commit_message>
PRINT USING for numerics as a start
</commit_message>
<xml_diff>
--- a/Supported.xlsx
+++ b/Supported.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/don/go/src/github.com/navionguy/basicwasm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FBF6FDE-3C13-BC4A-AC22-FDB49241CEC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA2CD2A-2EAD-BF4C-BDA8-B8BA02F6FD8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19000" xr2:uid="{AA62892B-5570-A74D-BDA8-A103E896D107}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="198">
   <si>
     <t>Functions, Commands &amp; Statement</t>
   </si>
@@ -626,6 +625,9 @@
   </si>
   <si>
     <t>cursor location only</t>
+  </si>
+  <si>
+    <t>Numerics only</t>
   </si>
 </sst>
 </file>
@@ -1031,10 +1033,10 @@
   <dimension ref="A1:L185"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="17280" ySplit="1800" topLeftCell="L147" activePane="bottomLeft"/>
+      <pane xSplit="17280" ySplit="1800" topLeftCell="L105" activePane="bottomLeft"/>
       <selection activeCell="B1" sqref="B1:B1048576"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="E177" sqref="E177"/>
+      <selection pane="bottomLeft" activeCell="G131" sqref="G131"/>
       <selection pane="bottomRight" activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
@@ -2297,6 +2299,18 @@
       <c r="A131" t="s">
         <v>136</v>
       </c>
+      <c r="C131" t="s">
+        <v>12</v>
+      </c>
+      <c r="D131" t="s">
+        <v>12</v>
+      </c>
+      <c r="E131" t="s">
+        <v>195</v>
+      </c>
+      <c r="G131" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
@@ -2789,15 +2803,15 @@
       </c>
       <c r="C184">
         <f>COUNTA(C2:C183)</f>
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D184">
         <f>COUNTA(D2:D183)</f>
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E184">
         <f>COUNTA(E2:E183)</f>
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.2">
@@ -2807,15 +2821,15 @@
       </c>
       <c r="C185" s="2">
         <f>C184/$A184</f>
-        <v>0.40109890109890112</v>
+        <v>0.40659340659340659</v>
       </c>
       <c r="D185" s="2">
         <f>D184/$A184</f>
-        <v>0.39560439560439559</v>
+        <v>0.40109890109890112</v>
       </c>
       <c r="E185" s="2">
         <f>E184/$A184</f>
-        <v>0.38461538461538464</v>
+        <v>0.39010989010989011</v>
       </c>
       <c r="F185" s="2"/>
     </row>

</xml_diff>

<commit_message>
how did I miss TAB()
</commit_message>
<xml_diff>
--- a/Supported.xlsx
+++ b/Supported.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/don/go/src/github.com/navionguy/basicwasm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA2CD2A-2EAD-BF4C-BDA8-B8BA02F6FD8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9D972EF-02E2-4546-95E0-D767511FF0AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19000" xr2:uid="{AA62892B-5570-A74D-BDA8-A103E896D107}"/>
+    <workbookView xWindow="35680" yWindow="1100" windowWidth="33600" windowHeight="19000" xr2:uid="{AA62892B-5570-A74D-BDA8-A103E896D107}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="200">
   <si>
     <t>Functions, Commands &amp; Statement</t>
   </si>
@@ -628,6 +628,12 @@
   </si>
   <si>
     <t>Numerics only</t>
+  </si>
+  <si>
+    <t>Not all params</t>
+  </si>
+  <si>
+    <t>Border color</t>
   </si>
 </sst>
 </file>
@@ -734,7 +740,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1022,7 +1028,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1033,10 +1039,10 @@
   <dimension ref="A1:L185"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="17280" ySplit="1800" topLeftCell="L105" activePane="bottomLeft"/>
+      <pane xSplit="17280" ySplit="1800" topLeftCell="L144" activePane="bottomLeft"/>
       <selection activeCell="B1" sqref="B1:B1048576"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="G131" sqref="G131"/>
+      <selection pane="bottomLeft" activeCell="G150" sqref="G150"/>
       <selection pane="bottomRight" activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
@@ -1213,6 +1219,15 @@
       <c r="A12" t="s">
         <v>16</v>
       </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -1320,6 +1335,9 @@
       <c r="D21" t="s">
         <v>12</v>
       </c>
+      <c r="E21" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
@@ -1580,6 +1598,15 @@
       <c r="A50" t="s">
         <v>55</v>
       </c>
+      <c r="C50" t="s">
+        <v>12</v>
+      </c>
+      <c r="D50" t="s">
+        <v>12</v>
+      </c>
+      <c r="E50" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
@@ -1807,6 +1834,18 @@
         <v>77</v>
       </c>
       <c r="B72" s="4"/>
+      <c r="C72" t="s">
+        <v>12</v>
+      </c>
+      <c r="D72" t="s">
+        <v>12</v>
+      </c>
+      <c r="E72" t="s">
+        <v>12</v>
+      </c>
+      <c r="G72" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
@@ -2388,6 +2427,15 @@
       <c r="A141" t="s">
         <v>146</v>
       </c>
+      <c r="C141" t="s">
+        <v>12</v>
+      </c>
+      <c r="D141" t="s">
+        <v>12</v>
+      </c>
+      <c r="E141" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
@@ -2425,7 +2473,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>150</v>
       </c>
@@ -2439,12 +2487,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>152</v>
       </c>
@@ -2458,12 +2506,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>154</v>
       </c>
@@ -2480,7 +2528,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A150" s="4" t="s">
         <v>155</v>
       </c>
@@ -2494,8 +2542,11 @@
       <c r="E150" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G150" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>157</v>
       </c>
@@ -2512,12 +2563,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>158</v>
       </c>
@@ -2534,12 +2585,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>160</v>
       </c>
@@ -2556,12 +2607,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>162</v>
       </c>
@@ -2578,12 +2629,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>164</v>
       </c>
@@ -2597,7 +2648,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>165</v>
       </c>
@@ -2649,6 +2700,18 @@
     <row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>170</v>
+      </c>
+      <c r="B165" t="s">
+        <v>12</v>
+      </c>
+      <c r="C165" t="s">
+        <v>12</v>
+      </c>
+      <c r="D165" t="s">
+        <v>12</v>
+      </c>
+      <c r="E165" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.2">
@@ -2799,37 +2862,37 @@
       </c>
       <c r="B184">
         <f>COUNTA(B2:B183)</f>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C184">
         <f>COUNTA(C2:C183)</f>
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="D184">
         <f>COUNTA(D2:D183)</f>
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="E184">
         <f>COUNTA(E2:E183)</f>
-        <v>71</v>
+        <v>77</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B185" s="2">
         <f>B184/$A184</f>
-        <v>0.18681318681318682</v>
+        <v>0.19230769230769232</v>
       </c>
       <c r="C185" s="2">
         <f>C184/$A184</f>
-        <v>0.40659340659340659</v>
+        <v>0.43406593406593408</v>
       </c>
       <c r="D185" s="2">
         <f>D184/$A184</f>
-        <v>0.40109890109890112</v>
+        <v>0.42857142857142855</v>
       </c>
       <c r="E185" s="2">
         <f>E184/$A184</f>
-        <v>0.39010989010989011</v>
+        <v>0.42307692307692307</v>
       </c>
       <c r="F185" s="2"/>
     </row>

</xml_diff>

<commit_message>
working on data file support
</commit_message>
<xml_diff>
--- a/Supported.xlsx
+++ b/Supported.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/don/go/src/github.com/navionguy/basicwasm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9D972EF-02E2-4546-95E0-D767511FF0AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C0E6401-5333-AF49-93D3-8E3BA9DF610A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="35680" yWindow="1100" windowWidth="33600" windowHeight="19000" xr2:uid="{AA62892B-5570-A74D-BDA8-A103E896D107}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="200">
   <si>
     <t>Functions, Commands &amp; Statement</t>
   </si>
@@ -740,7 +740,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1028,7 +1028,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1039,10 +1039,10 @@
   <dimension ref="A1:L185"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="17280" ySplit="1800" topLeftCell="L144" activePane="bottomLeft"/>
+      <pane xSplit="17280" ySplit="1800" topLeftCell="L33" activePane="bottomLeft"/>
       <selection activeCell="B1" sqref="B1:B1048576"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="G150" sqref="G150"/>
+      <selection pane="bottomLeft" activeCell="E111" sqref="E111"/>
       <selection pane="bottomRight" activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
@@ -2217,10 +2217,25 @@
       <c r="A111" t="s">
         <v>116</v>
       </c>
+      <c r="C111" t="s">
+        <v>12</v>
+      </c>
+      <c r="D111" t="s">
+        <v>12</v>
+      </c>
+      <c r="E111" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>117</v>
+      </c>
+      <c r="C112" t="s">
+        <v>12</v>
+      </c>
+      <c r="D112" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
@@ -2866,15 +2881,15 @@
       </c>
       <c r="C184">
         <f>COUNTA(C2:C183)</f>
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D184">
         <f>COUNTA(D2:D183)</f>
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E184">
         <f>COUNTA(E2:E183)</f>
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.2">
@@ -2884,15 +2899,15 @@
       </c>
       <c r="C185" s="2">
         <f>C184/$A184</f>
-        <v>0.43406593406593408</v>
+        <v>0.44505494505494503</v>
       </c>
       <c r="D185" s="2">
         <f>D184/$A184</f>
-        <v>0.42857142857142855</v>
+        <v>0.43956043956043955</v>
       </c>
       <c r="E185" s="2">
         <f>E184/$A184</f>
-        <v>0.42307692307692307</v>
+        <v>0.42857142857142855</v>
       </c>
       <c r="F185" s="2"/>
     </row>

</xml_diff>

<commit_message>
error handling and test coverage
</commit_message>
<xml_diff>
--- a/Supported.xlsx
+++ b/Supported.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/don/go/src/github.com/navionguy/basicwasm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C0E6401-5333-AF49-93D3-8E3BA9DF610A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5131EA0C-A7A8-7549-8140-9CA126035238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35680" yWindow="1100" windowWidth="33600" windowHeight="19000" xr2:uid="{AA62892B-5570-A74D-BDA8-A103E896D107}"/>
+    <workbookView xWindow="57240" yWindow="2720" windowWidth="31140" windowHeight="19000" xr2:uid="{AA62892B-5570-A74D-BDA8-A103E896D107}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1039,7 +1040,7 @@
   <dimension ref="A1:L185"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="17280" ySplit="1800" topLeftCell="L33" activePane="bottomLeft"/>
+      <pane xSplit="17280" ySplit="1800" topLeftCell="L1" activePane="bottomLeft"/>
       <selection activeCell="B1" sqref="B1:B1048576"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="E111" sqref="E111"/>

</xml_diff>